<commit_message>
first rule implemented. tests to be implemented.
</commit_message>
<xml_diff>
--- a/validator/resources/OntoUML Rules.xlsx
+++ b/validator/resources/OntoUML Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FavatoBarcelosPP\Dev\ontouml-validator\validator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6542C390-D167-41C9-9902-59C8B6A96EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF6996E-4A49-43B3-98F4-5A4BA3D53099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2464,7 +2464,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="C6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
rules py file separated into general and individual. rule CL001 implemented. Tests working. pre-commit reactivated. workflows adjusted
</commit_message>
<xml_diff>
--- a/validator/resources/OntoUML Rules.xlsx
+++ b/validator/resources/OntoUML Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FavatoBarcelosPP\Dev\ontouml-validator\validator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12576737-D842-4F5F-85D6-266501D62537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C60070B-5425-4ACF-81FC-C8E4000CF70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules Definition" sheetId="2" r:id="rId1"/>
@@ -450,9 +450,6 @@
     <t>Rule Description</t>
   </si>
   <si>
-    <t>Situation Number</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -508,6 +505,9 @@
   </si>
   <si>
     <t>Two stereotypes for the same class is not currently supported by the exporting tool. Tests was adjusted manually.</t>
+  </si>
+  <si>
+    <t>Situation ID</t>
   </si>
 </sst>
 </file>
@@ -642,6 +642,12 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C5700"/>
       </font>
@@ -690,12 +696,6 @@
           <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -845,9 +845,9 @@
     <tableColumn id="2" xr3:uid="{65D02219-A7C8-4BC4-BE70-FC12D26642C7}" name="Rule Description" dataDxfId="9">
       <calculatedColumnFormula>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{39BF0221-09C6-4746-A9C6-D71D4B6C7533}" name="Situation Number"/>
+    <tableColumn id="5" xr3:uid="{39BF0221-09C6-4746-A9C6-D71D4B6C7533}" name="Situation ID"/>
     <tableColumn id="6" xr3:uid="{FE3246A6-E21A-441F-A08A-12268F822A02}" name="Situation Code" dataDxfId="8">
-      <calculatedColumnFormula>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation Number]]</calculatedColumnFormula>
+      <calculatedColumnFormula>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{ED1E7C03-7BE4-4AD0-867B-6CF8D46CE033}" name="Test File" dataDxfId="7">
       <calculatedColumnFormula>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</calculatedColumnFormula>
@@ -855,11 +855,11 @@
     <tableColumn id="3" xr3:uid="{F491E82A-09B4-4B22-AA08-7E6DFD336A64}" name="Situation Description"/>
     <tableColumn id="4" xr3:uid="{92BCF063-80EB-4A9C-AA1A-6F95CC9435A7}" name="OWA Level"/>
     <tableColumn id="7" xr3:uid="{DB4F2106-6953-489A-AB24-1163C09441FE}" name="CWA Level"/>
-    <tableColumn id="10" xr3:uid="{E91C3898-466B-4A4C-8CF6-E0B90D5094B2}" name="Test OWA Entry" dataDxfId="6">
-      <calculatedColumnFormula>"owa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{E91C3898-466B-4A4C-8CF6-E0B90D5094B2}" name="Test OWA Entry" dataDxfId="1">
+      <calculatedColumnFormula>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D99049E8-95AA-440A-B6C3-AB032C08C4B8}" name="Test CWA Entry" dataDxfId="5">
-      <calculatedColumnFormula>"cwa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{D99049E8-95AA-440A-B6C3-AB032C08C4B8}" name="Test CWA Entry" dataDxfId="0">
+      <calculatedColumnFormula>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{9CF1643D-B8F2-452E-B29E-AD6EF72070C4}" name="Comments"/>
   </tableColumns>
@@ -1218,7 +1218,7 @@
         <v>CL001</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>2</v>
@@ -2409,7 +2409,7 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="C2:C78">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2431,20 +2431,21 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="100.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="80.7109375" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="104" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2456,13 +2457,13 @@
         <v>137</v>
       </c>
       <c r="C1" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="D1" t="s">
         <v>132</v>
       </c>
       <c r="E1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F1" t="s">
         <v>136</v>
@@ -2471,16 +2472,16 @@
         <v>81</v>
       </c>
       <c r="H1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" t="s">
         <v>154</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>155</v>
-      </c>
-      <c r="K1" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2492,10 +2493,10 @@
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D2" s="10" t="str">
-        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation Number]]</f>
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
         <v>CL001A</v>
       </c>
       <c r="E2" s="10" t="str">
@@ -2512,12 +2513,12 @@
         <v>135</v>
       </c>
       <c r="I2" t="str">
-        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
-        <v>owa,CL001A.ttl,warning</v>
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL001,CL001A.ttl,warning</v>
       </c>
       <c r="J2" t="str">
-        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
-        <v>cwa,CL001A.ttl,error</v>
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL001,CL001A.ttl,error</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2529,10 +2530,10 @@
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation Number]]</f>
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
         <v>CL001B</v>
       </c>
       <c r="E3" s="10" t="str">
@@ -2540,21 +2541,21 @@
         <v>CL001B.ttl</v>
       </c>
       <c r="F3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I3" t="str">
-        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
-        <v>owa,CL001B.ttl,valid</v>
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL001,CL001B.ttl,valid</v>
       </c>
       <c r="J3" t="str">
-        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
-        <v>cwa,CL001B.ttl,valid</v>
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL001,CL001B.ttl,valid</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2566,10 +2567,10 @@
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D4" s="10" t="str">
-        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation Number]]</f>
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
         <v>CL001C</v>
       </c>
       <c r="E4" s="10" t="str">
@@ -2577,21 +2578,21 @@
         <v>CL001C.ttl</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I4" t="str">
-        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
-        <v>owa,CL001C.ttl,valid</v>
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL001,CL001C.ttl,valid</v>
       </c>
       <c r="J4" t="str">
-        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
-        <v>cwa,CL001C.ttl,valid</v>
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL001,CL001C.ttl,valid</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2603,10 +2604,10 @@
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D5" t="str">
-        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation Number]]</f>
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
         <v>CL001D</v>
       </c>
       <c r="E5" t="str">
@@ -2614,7 +2615,7 @@
         <v>CL001D.ttl</v>
       </c>
       <c r="F5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G5" t="s">
         <v>135</v>
@@ -2623,15 +2624,15 @@
         <v>135</v>
       </c>
       <c r="I5" t="str">
-        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
-        <v>owa,CL001D.ttl,error</v>
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL001,CL001D.ttl,error</v>
       </c>
       <c r="J5" t="str">
-        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
-        <v>cwa,CL001D.ttl,error</v>
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL001,CL001D.ttl,error</v>
       </c>
       <c r="K5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2643,10 +2644,10 @@
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D6" t="str">
-        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation Number]]</f>
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
         <v>CL001E</v>
       </c>
       <c r="E6" t="str">
@@ -2654,7 +2655,7 @@
         <v>CL001E.ttl</v>
       </c>
       <c r="F6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G6" t="s">
         <v>135</v>
@@ -2663,15 +2664,15 @@
         <v>135</v>
       </c>
       <c r="I6" t="str">
-        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
-        <v>owa,CL001E.ttl,error</v>
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL001,CL001E.ttl,error</v>
       </c>
       <c r="J6" t="str">
-        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
-        <v>cwa,CL001E.ttl,error</v>
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL001,CL001E.ttl,error</v>
       </c>
       <c r="K6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2683,10 +2684,10 @@
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D7" t="str">
-        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation Number]]</f>
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
         <v>CL001F</v>
       </c>
       <c r="E7" t="str">
@@ -2694,7 +2695,7 @@
         <v>CL001F.ttl</v>
       </c>
       <c r="F7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G7" t="s">
         <v>135</v>
@@ -2703,29 +2704,29 @@
         <v>135</v>
       </c>
       <c r="I7" t="str">
-        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
-        <v>owa,CL001F.ttl,error</v>
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL001,CL001F.ttl,error</v>
       </c>
       <c r="J7" t="str">
-        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
-        <v>cwa,CL001F.ttl,error</v>
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL001,CL001F.ttl,error</v>
       </c>
       <c r="K7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:E7">
-    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:H7">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Valid"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add CL003 test files
</commit_message>
<xml_diff>
--- a/validator/resources/OntoUML Rules.xlsx
+++ b/validator/resources/OntoUML Rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FavatoBarcelosPP\Dev\ontouml-validator\validator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D00A568-51F1-4E88-B280-5CB45F2BF864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDE2C85-D074-4954-8AEC-2784A3368332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="167">
   <si>
     <t>Source Element</t>
   </si>
@@ -511,6 +511,30 @@
   </si>
   <si>
     <t>CL002</t>
+  </si>
+  <si>
+    <t>enumerations must have literals</t>
+  </si>
+  <si>
+    <t>CL003</t>
+  </si>
+  <si>
+    <t>Class that is not an enumeration without attributes</t>
+  </si>
+  <si>
+    <t>Class that is not an enumeration with one attribute</t>
+  </si>
+  <si>
+    <t>Class that is an enumeration with one attribute</t>
+  </si>
+  <si>
+    <t>Class that is an enumeration without attributes</t>
+  </si>
+  <si>
+    <t>Class that is an enumeration with two attributes</t>
+  </si>
+  <si>
+    <t>Class that is not an enumeration with two attributes</t>
   </si>
 </sst>
 </file>
@@ -644,7 +668,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="52">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -727,6 +751,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -762,6 +806,246 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -896,15 +1180,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}" name="TabRules" displayName="TabRules" ref="A1:D78" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}" name="TabRules" displayName="TabRules" ref="A1:D78" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A1:D78" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{F9D36F48-DD19-43E5-A1AB-8357F96419FF}" name="Source Element" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{1DEB1013-754C-4E97-AF35-6F79DD0210E4}" name="Group Number" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{05F466FD-E5DB-4DED-979E-C9E29087B8F6}" name="Rule Code" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{F9D36F48-DD19-43E5-A1AB-8357F96419FF}" name="Source Element" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{1DEB1013-754C-4E97-AF35-6F79DD0210E4}" name="Group Number" dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{05F466FD-E5DB-4DED-979E-C9E29087B8F6}" name="Rule Code" dataDxfId="47">
       <calculatedColumnFormula>VLOOKUP(TabRules[[#This Row],[Source Element]],TabGroups[#All],2,FALSE)&amp;TabRules[[#This Row],[Group Number]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{70BA6684-6E4A-40D9-BE42-830C46F4D6A9}" name="Description" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{70BA6684-6E4A-40D9-BE42-830C46F4D6A9}" name="Description" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -914,7 +1198,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D8A1ADE-544A-443A-AF20-52BBCA41FA15}" name="TabGroups" displayName="TabGroups" ref="F1:G6" totalsRowShown="0">
   <autoFilter ref="F1:G6" xr:uid="{3D8A1ADE-544A-443A-AF20-52BBCA41FA15}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2E543EF0-9E26-4478-A5D0-A70AC90899EE}" name="Source Element" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{2E543EF0-9E26-4478-A5D0-A70AC90899EE}" name="Source Element" dataDxfId="45"/>
     <tableColumn id="2" xr3:uid="{2A3CE154-AB6B-45C3-B5E2-2E1AC49C63C7}" name="Code"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -922,27 +1206,27 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}" name="TabImp" displayName="TabImp" ref="A1:K13" totalsRowShown="0">
-  <autoFilter ref="A1:K13" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}" name="TabImp" displayName="TabImp" ref="A1:K19" totalsRowShown="0">
+  <autoFilter ref="A1:K19" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5662254C-D4AB-4E75-B315-CAFCAA30EDF4}" name="Rule Code" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{65D02219-A7C8-4BC4-BE70-FC12D26642C7}" name="Rule Description" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{5662254C-D4AB-4E75-B315-CAFCAA30EDF4}" name="Rule Code" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{65D02219-A7C8-4BC4-BE70-FC12D26642C7}" name="Rule Description" dataDxfId="43">
       <calculatedColumnFormula>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{39BF0221-09C6-4746-A9C6-D71D4B6C7533}" name="Situation ID"/>
-    <tableColumn id="6" xr3:uid="{FE3246A6-E21A-441F-A08A-12268F822A02}" name="Situation Code" dataDxfId="16">
+    <tableColumn id="6" xr3:uid="{FE3246A6-E21A-441F-A08A-12268F822A02}" name="Situation Code" dataDxfId="42">
       <calculatedColumnFormula>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ED1E7C03-7BE4-4AD0-867B-6CF8D46CE033}" name="Test File" dataDxfId="15">
+    <tableColumn id="8" xr3:uid="{ED1E7C03-7BE4-4AD0-867B-6CF8D46CE033}" name="Test File" dataDxfId="41">
       <calculatedColumnFormula>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{F491E82A-09B4-4B22-AA08-7E6DFD336A64}" name="Situation Description"/>
     <tableColumn id="4" xr3:uid="{92BCF063-80EB-4A9C-AA1A-6F95CC9435A7}" name="OWA Level"/>
     <tableColumn id="7" xr3:uid="{DB4F2106-6953-489A-AB24-1163C09441FE}" name="CWA Level"/>
-    <tableColumn id="10" xr3:uid="{E91C3898-466B-4A4C-8CF6-E0B90D5094B2}" name="Test OWA Entry" dataDxfId="14">
+    <tableColumn id="10" xr3:uid="{E91C3898-466B-4A4C-8CF6-E0B90D5094B2}" name="Test OWA Entry" dataDxfId="40">
       <calculatedColumnFormula>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D99049E8-95AA-440A-B6C3-AB032C08C4B8}" name="Test CWA Entry" dataDxfId="13">
+    <tableColumn id="11" xr3:uid="{D99049E8-95AA-440A-B6C3-AB032C08C4B8}" name="Test CWA Entry" dataDxfId="39">
       <calculatedColumnFormula>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{9CF1643D-B8F2-452E-B29E-AD6EF72070C4}" name="Comments"/>
@@ -1251,11 +1535,11 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G83"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2490,10 +2774,18 @@
         <v>90</v>
       </c>
     </row>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="C2:C78">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D78">
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -2511,11 +2803,11 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,7 +2816,7 @@
     <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="65" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -3030,23 +3322,245 @@
         <v>156</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="12" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
+      </c>
+      <c r="C14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL003A</v>
+      </c>
+      <c r="E14" s="12" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL003A.ttl</v>
+      </c>
+      <c r="F14" t="s">
+        <v>161</v>
+      </c>
+      <c r="G14" t="s">
+        <v>140</v>
+      </c>
+      <c r="H14" t="s">
+        <v>140</v>
+      </c>
+      <c r="I14" s="12" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL003,CL003A.ttl,valid</v>
+      </c>
+      <c r="J14" s="12" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL003,CL003A.ttl,valid</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="12" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
+      </c>
+      <c r="C15" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL003B</v>
+      </c>
+      <c r="E15" s="12" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL003B.ttl</v>
+      </c>
+      <c r="F15" t="s">
+        <v>162</v>
+      </c>
+      <c r="G15" t="s">
+        <v>140</v>
+      </c>
+      <c r="H15" t="s">
+        <v>140</v>
+      </c>
+      <c r="I15" s="12" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL003,CL003B.ttl,valid</v>
+      </c>
+      <c r="J15" s="12" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL003,CL003B.ttl,valid</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="12" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
+      </c>
+      <c r="C16" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL003C</v>
+      </c>
+      <c r="E16" s="12" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL003C.ttl</v>
+      </c>
+      <c r="F16" t="s">
+        <v>166</v>
+      </c>
+      <c r="G16" t="s">
+        <v>140</v>
+      </c>
+      <c r="H16" t="s">
+        <v>140</v>
+      </c>
+      <c r="I16" s="12" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL003,CL003C.ttl,valid</v>
+      </c>
+      <c r="J16" s="12" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL003,CL003C.ttl,valid</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="12" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
+      </c>
+      <c r="C17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL003D</v>
+      </c>
+      <c r="E17" s="12" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL003D.ttl</v>
+      </c>
+      <c r="F17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G17" t="s">
+        <v>140</v>
+      </c>
+      <c r="H17" t="s">
+        <v>140</v>
+      </c>
+      <c r="I17" s="12" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL003,CL003D.ttl,valid</v>
+      </c>
+      <c r="J17" s="12" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL003,CL003D.ttl,valid</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B18" s="12" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
+      </c>
+      <c r="C18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL003E</v>
+      </c>
+      <c r="E18" s="12" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL003E.ttl</v>
+      </c>
+      <c r="F18" t="s">
+        <v>163</v>
+      </c>
+      <c r="G18" t="s">
+        <v>135</v>
+      </c>
+      <c r="H18" t="s">
+        <v>135</v>
+      </c>
+      <c r="I18" s="12" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL003,CL003E.ttl,error</v>
+      </c>
+      <c r="J18" s="12" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL003,CL003E.ttl,error</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B19" s="12" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
+      </c>
+      <c r="C19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="12" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL003F</v>
+      </c>
+      <c r="E19" s="12" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL003F.ttl</v>
+      </c>
+      <c r="F19" t="s">
+        <v>165</v>
+      </c>
+      <c r="G19" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" t="s">
+        <v>135</v>
+      </c>
+      <c r="I19" s="12" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL003,CL003F.ttl,error</v>
+      </c>
+      <c r="J19" s="12" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL003,CL003F.ttl,error</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:E13">
-    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+  <conditionalFormatting sqref="D2:E19">
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H13">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
+  <conditionalFormatting sqref="G2:H19">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Valid"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H13" xr:uid="{88F4C713-6BF6-49A8-982F-7D1643817146}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H19" xr:uid="{88F4C713-6BF6-49A8-982F-7D1643817146}">
       <formula1>"Valid,Error,Warning"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
rules CL_EN_01 and CL_EN_02 working
</commit_message>
<xml_diff>
--- a/validator/resources/OntoUML Rules.xlsx
+++ b/validator/resources/OntoUML Rules.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FavatoBarcelosPP\Dev\ontouml-validator\validator\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0685DB9-FE4F-4D81-B4C2-AD3506CB46B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B238CD54-C486-434E-B76D-F3C5463C8DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rules Definition" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="152">
   <si>
     <t>Description</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Every class decorated with the stereotype «enumeration» must not have attributes.</t>
   </si>
   <si>
-    <t>Every class having enumeration literals must be decorated with the stereotype «enumeration».</t>
-  </si>
-  <si>
     <t>Every class decorated with a base sortal stereotype (i.e., «subkind», «phase», «role», or «historicalRole») must specialize a unique class decorated with a ultimate sortal stereotype (i.e., «kind», «collective», «quantity», «relator», «mode», «quality», or «type»).</t>
   </si>
   <si>
@@ -463,6 +460,36 @@
   </si>
   <si>
     <t>Enumeration classes cannot be generalized by classes with stereotype Abstract.</t>
+  </si>
+  <si>
+    <t>CL_EN_02</t>
+  </si>
+  <si>
+    <t>Class that is an enumeration without literals</t>
+  </si>
+  <si>
+    <t>Class that is an enumeration with one enumeration literal</t>
+  </si>
+  <si>
+    <t>Created manually as it is not possible to export from VP.</t>
+  </si>
+  <si>
+    <t>Every class having enumeration literals must be decorated with the stereotype enumeration.</t>
+  </si>
+  <si>
+    <t>Class with stereptype different from enumeration without literals</t>
+  </si>
+  <si>
+    <t>Class with stereptype different from enumeration with one enumeration literal</t>
+  </si>
+  <si>
+    <t>Manually created.</t>
+  </si>
+  <si>
+    <t>Class without stereotype without literals</t>
+  </si>
+  <si>
+    <t>Class without stereotype that has with one enumeration literal</t>
   </si>
 </sst>
 </file>
@@ -564,7 +591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -605,11 +632,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="45">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -617,6 +655,216 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -870,26 +1118,6 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <sz val="10"/>
@@ -912,56 +1140,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}" name="TabRules" displayName="TabRules" ref="A1:E80" totalsRowShown="0" headerRowDxfId="24" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}" name="TabRules" displayName="TabRules" ref="A1:E80" totalsRowShown="0" headerRowDxfId="44" dataDxfId="32">
   <autoFilter ref="A1:E80" xr:uid="{198E5AA4-A716-476C-94EA-BE3270ADAC25}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{F9D36F48-DD19-43E5-A1AB-8357F96419FF}" name="Group" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{92D3A8C7-5541-45DC-A40E-AED787463128}" name="SubGroup" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{1DEB1013-754C-4E97-AF35-6F79DD0210E4}" name="Group Number" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{05F466FD-E5DB-4DED-979E-C9E29087B8F6}" name="Rule Code" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{F9D36F48-DD19-43E5-A1AB-8357F96419FF}" name="Group" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{92D3A8C7-5541-45DC-A40E-AED787463128}" name="SubGroup" dataDxfId="36"/>
+    <tableColumn id="6" xr3:uid="{1DEB1013-754C-4E97-AF35-6F79DD0210E4}" name="Group Number" dataDxfId="35"/>
+    <tableColumn id="7" xr3:uid="{05F466FD-E5DB-4DED-979E-C9E29087B8F6}" name="Rule Code" dataDxfId="34">
       <calculatedColumnFormula>VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;VLOOKUP(TabRules[[#This Row],[SubGroup]],TabGroups[[#All],[Subgroup]:[Subgroup Code]],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[Group Number]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{70BA6684-6E4A-40D9-BE42-830C46F4D6A9}" name="Description" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{70BA6684-6E4A-40D9-BE42-830C46F4D6A9}" name="Description" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D8A1ADE-544A-443A-AF20-52BBCA41FA15}" name="TabGroups" displayName="TabGroups" ref="G1:J6" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{3D8A1ADE-544A-443A-AF20-52BBCA41FA15}" name="TabGroups" displayName="TabGroups" ref="G1:J6" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="G1:J6" xr:uid="{3D8A1ADE-544A-443A-AF20-52BBCA41FA15}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2E543EF0-9E26-4478-A5D0-A70AC90899EE}" name="Group" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{2A3CE154-AB6B-45C3-B5E2-2E1AC49C63C7}" name="Group Code" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{598019D5-4069-412F-A57E-586DD6241ACC}" name="Subgroup" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{90E1C2A9-5C06-48CB-A78C-54E7D56B3BFC}" name="Subgroup Code" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{2E543EF0-9E26-4478-A5D0-A70AC90899EE}" name="Group" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{2A3CE154-AB6B-45C3-B5E2-2E1AC49C63C7}" name="Group Code" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{598019D5-4069-412F-A57E-586DD6241ACC}" name="Subgroup" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{90E1C2A9-5C06-48CB-A78C-54E7D56B3BFC}" name="Subgroup Code" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}" name="TabImp" displayName="TabImp" ref="A1:K19" totalsRowShown="0">
-  <autoFilter ref="A1:K19" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}" name="TabImp" displayName="TabImp" ref="A1:K25" totalsRowShown="0">
+  <autoFilter ref="A1:K25" xr:uid="{677213A8-3C35-46A4-83EE-9953AF366E80}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{5662254C-D4AB-4E75-B315-CAFCAA30EDF4}" name="Rule Code" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{65D02219-A7C8-4BC4-BE70-FC12D26642C7}" name="Rule Description" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{5662254C-D4AB-4E75-B315-CAFCAA30EDF4}" name="Rule Code" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{65D02219-A7C8-4BC4-BE70-FC12D26642C7}" name="Rule Description" dataDxfId="18">
       <calculatedColumnFormula>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{39BF0221-09C6-4746-A9C6-D71D4B6C7533}" name="Situation ID"/>
-    <tableColumn id="6" xr3:uid="{FE3246A6-E21A-441F-A08A-12268F822A02}" name="Situation Code" dataDxfId="21">
+    <tableColumn id="6" xr3:uid="{FE3246A6-E21A-441F-A08A-12268F822A02}" name="Situation Code" dataDxfId="17">
       <calculatedColumnFormula>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{ED1E7C03-7BE4-4AD0-867B-6CF8D46CE033}" name="Test File" dataDxfId="20">
+    <tableColumn id="8" xr3:uid="{ED1E7C03-7BE4-4AD0-867B-6CF8D46CE033}" name="Test File" dataDxfId="16">
       <calculatedColumnFormula>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{F491E82A-09B4-4B22-AA08-7E6DFD336A64}" name="Situation Description"/>
     <tableColumn id="4" xr3:uid="{92BCF063-80EB-4A9C-AA1A-6F95CC9435A7}" name="OWA Level"/>
     <tableColumn id="7" xr3:uid="{DB4F2106-6953-489A-AB24-1163C09441FE}" name="CWA Level"/>
-    <tableColumn id="10" xr3:uid="{E91C3898-466B-4A4C-8CF6-E0B90D5094B2}" name="Test OWA Entry" dataDxfId="19">
+    <tableColumn id="10" xr3:uid="{E91C3898-466B-4A4C-8CF6-E0B90D5094B2}" name="Test OWA Entry" dataDxfId="15">
       <calculatedColumnFormula>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D99049E8-95AA-440A-B6C3-AB032C08C4B8}" name="Test CWA Entry" dataDxfId="18">
+    <tableColumn id="11" xr3:uid="{D99049E8-95AA-440A-B6C3-AB032C08C4B8}" name="Test CWA Entry" dataDxfId="14">
       <calculatedColumnFormula>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{9CF1643D-B8F2-452E-B29E-AD6EF72070C4}" name="Comments"/>
@@ -1272,9 +1500,9 @@
   </sheetPr>
   <dimension ref="A1:J85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1294,31 +1522,31 @@
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1326,29 +1554,29 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="D2" s="14" t="str">
+        <f>VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;VLOOKUP(TabRules[[#This Row],[SubGroup]],TabGroups[[#All],[Subgroup]:[Subgroup Code]],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[Group Number]]</f>
+        <v>CL_ST_01</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" s="14" t="str">
-        <f>VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;VLOOKUP(TabRules[[#This Row],[SubGroup]],TabGroups[[#All],[Subgroup]:[Subgroup Code]],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[Group Number]]</f>
-        <v>CL_ST_01</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1356,10 +1584,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D3" s="14" t="str">
         <f>VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;VLOOKUP(TabRules[[#This Row],[SubGroup]],TabGroups[[#All],[Subgroup]:[Subgroup Code]],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[Group Number]]</f>
@@ -1369,16 +1597,16 @@
         <v>2</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1386,10 +1614,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D4" s="14" t="str">
         <f>VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;VLOOKUP(TabRules[[#This Row],[SubGroup]],TabGroups[[#All],[Subgroup]:[Subgroup Code]],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[Group Number]]</f>
@@ -1399,10 +1627,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="11"/>
@@ -1412,23 +1640,23 @@
         <v>1</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D5" s="14" t="str">
         <f>VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;VLOOKUP(TabRules[[#This Row],[SubGroup]],TabGroups[[#All],[Subgroup]:[Subgroup Code]],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[Group Number]]</f>
         <v>CL_EN_02</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>4</v>
+        <v>146</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I5" s="10"/>
       <c r="J5" s="11"/>
@@ -1438,23 +1666,23 @@
         <v>1</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D6" s="14" t="str">
         <f>VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;VLOOKUP(TabRules[[#This Row],[SubGroup]],TabGroups[[#All],[Subgroup]:[Subgroup Code]],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[Group Number]]</f>
         <v>CL_EN_03</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="11"/>
@@ -1464,17 +1692,17 @@
         <v>1</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D7" s="14" t="str">
         <f>VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;VLOOKUP(TabRules[[#This Row],[SubGroup]],TabGroups[[#All],[Subgroup]:[Subgroup Code]],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[Group Number]]</f>
         <v>CL_EN_04</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7"/>
@@ -1484,17 +1712,17 @@
         <v>1</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="15" t="str">
+        <f>VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;VLOOKUP(TabRules[[#This Row],[SubGroup]],TabGroups[[#All],[Subgroup]:[Subgroup Code]],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[Group Number]]</f>
+        <v>CL_EN_05</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>141</v>
-      </c>
-      <c r="D8" s="15" t="str">
-        <f>VLOOKUP(TabRules[[#This Row],[Group]],TabGroups[#All],2,FALSE)&amp;"_"&amp;VLOOKUP(TabRules[[#This Row],[SubGroup]],TabGroups[[#All],[Subgroup]:[Subgroup Code]],2,FALSE)&amp;"_"&amp;TabRules[[#This Row],[Group Number]]</f>
-        <v>CL_EN_05</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1508,7 +1736,7 @@
         <v>#N/A</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1522,7 +1750,7 @@
         <v>#N/A</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1536,7 +1764,7 @@
         <v>#N/A</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1550,7 +1778,7 @@
         <v>#N/A</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1564,7 +1792,7 @@
         <v>#N/A</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1578,7 +1806,7 @@
         <v>#N/A</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1592,7 +1820,7 @@
         <v>#N/A</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1606,7 +1834,7 @@
         <v>#N/A</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1620,7 +1848,7 @@
         <v>#N/A</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1634,7 +1862,7 @@
         <v>#N/A</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1648,7 +1876,7 @@
         <v>#N/A</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1662,7 +1890,7 @@
         <v>#N/A</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1676,7 +1904,7 @@
         <v>#N/A</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1690,7 +1918,7 @@
         <v>#N/A</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1704,7 +1932,7 @@
         <v>#N/A</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1718,7 +1946,7 @@
         <v>#N/A</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1732,7 +1960,7 @@
         <v>#N/A</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1746,7 +1974,7 @@
         <v>#N/A</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1760,7 +1988,7 @@
         <v>#N/A</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1774,7 +2002,7 @@
         <v>#N/A</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1788,7 +2016,7 @@
         <v>#N/A</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1802,7 +2030,7 @@
         <v>#N/A</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1816,7 +2044,7 @@
         <v>#N/A</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1830,7 +2058,7 @@
         <v>#N/A</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1844,7 +2072,7 @@
         <v>#N/A</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1858,7 +2086,7 @@
         <v>#N/A</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1872,7 +2100,7 @@
         <v>#N/A</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1886,7 +2114,7 @@
         <v>#N/A</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1900,7 +2128,7 @@
         <v>#N/A</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1914,7 +2142,7 @@
         <v>#N/A</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1928,7 +2156,7 @@
         <v>#N/A</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1942,7 +2170,7 @@
         <v>#N/A</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1956,7 +2184,7 @@
         <v>#N/A</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1970,12 +2198,12 @@
         <v>#N/A</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" s="12"/>
       <c r="C43" s="13"/>
@@ -1984,12 +2212,12 @@
         <v>#N/A</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="12"/>
       <c r="C44" s="13"/>
@@ -1998,12 +2226,12 @@
         <v>#N/A</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="12"/>
       <c r="C45" s="13"/>
@@ -2012,12 +2240,12 @@
         <v>#N/A</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" s="12"/>
       <c r="C46" s="13"/>
@@ -2026,12 +2254,12 @@
         <v>#N/A</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" s="12"/>
       <c r="C47" s="13"/>
@@ -2040,12 +2268,12 @@
         <v>#N/A</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B48" s="12"/>
       <c r="C48" s="13"/>
@@ -2054,12 +2282,12 @@
         <v>#N/A</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B49" s="12"/>
       <c r="C49" s="13"/>
@@ -2068,12 +2296,12 @@
         <v>#N/A</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" s="12"/>
       <c r="C50" s="13"/>
@@ -2082,12 +2310,12 @@
         <v>#N/A</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B51" s="12"/>
       <c r="C51" s="13"/>
@@ -2096,12 +2324,12 @@
         <v>#N/A</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B52" s="12"/>
       <c r="C52" s="13"/>
@@ -2110,12 +2338,12 @@
         <v>#N/A</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B53" s="12"/>
       <c r="C53" s="13"/>
@@ -2124,12 +2352,12 @@
         <v>#N/A</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B54" s="12"/>
       <c r="C54" s="13"/>
@@ -2138,12 +2366,12 @@
         <v>#N/A</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B55" s="12"/>
       <c r="C55" s="13"/>
@@ -2152,12 +2380,12 @@
         <v>#N/A</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B56" s="12"/>
       <c r="C56" s="13"/>
@@ -2166,12 +2394,12 @@
         <v>#N/A</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B57" s="12"/>
       <c r="C57" s="13"/>
@@ -2180,12 +2408,12 @@
         <v>#N/A</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B58" s="12"/>
       <c r="C58" s="13"/>
@@ -2194,12 +2422,12 @@
         <v>#N/A</v>
       </c>
       <c r="E58" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B59" s="12"/>
       <c r="C59" s="13"/>
@@ -2208,12 +2436,12 @@
         <v>#N/A</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="13"/>
@@ -2222,12 +2450,12 @@
         <v>#N/A</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B61" s="12"/>
       <c r="C61" s="13"/>
@@ -2236,12 +2464,12 @@
         <v>#N/A</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="13"/>
@@ -2250,12 +2478,12 @@
         <v>#N/A</v>
       </c>
       <c r="E62" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="13"/>
@@ -2264,12 +2492,12 @@
         <v>#N/A</v>
       </c>
       <c r="E63" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="13"/>
@@ -2278,12 +2506,12 @@
         <v>#N/A</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B65" s="12"/>
       <c r="C65" s="13"/>
@@ -2292,12 +2520,12 @@
         <v>#N/A</v>
       </c>
       <c r="E65" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B66" s="12"/>
       <c r="C66" s="13"/>
@@ -2306,12 +2534,12 @@
         <v>#N/A</v>
       </c>
       <c r="E66" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B67" s="12"/>
       <c r="C67" s="13"/>
@@ -2320,12 +2548,12 @@
         <v>#N/A</v>
       </c>
       <c r="E67" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B68" s="12"/>
       <c r="C68" s="13"/>
@@ -2334,12 +2562,12 @@
         <v>#N/A</v>
       </c>
       <c r="E68" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B69" s="12"/>
       <c r="C69" s="13"/>
@@ -2348,12 +2576,12 @@
         <v>#N/A</v>
       </c>
       <c r="E69" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B70" s="12"/>
       <c r="C70" s="13"/>
@@ -2362,12 +2590,12 @@
         <v>#N/A</v>
       </c>
       <c r="E70" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B71" s="12"/>
       <c r="C71" s="13"/>
@@ -2376,12 +2604,12 @@
         <v>#N/A</v>
       </c>
       <c r="E71" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B72" s="12"/>
       <c r="C72" s="13"/>
@@ -2390,12 +2618,12 @@
         <v>#N/A</v>
       </c>
       <c r="E72" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B73" s="12"/>
       <c r="C73" s="13"/>
@@ -2404,12 +2632,12 @@
         <v>#N/A</v>
       </c>
       <c r="E73" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B74" s="12"/>
       <c r="C74" s="13"/>
@@ -2418,12 +2646,12 @@
         <v>#N/A</v>
       </c>
       <c r="E74" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B75" s="12"/>
       <c r="C75" s="13"/>
@@ -2432,12 +2660,12 @@
         <v>#N/A</v>
       </c>
       <c r="E75" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B76" s="12"/>
       <c r="C76" s="13"/>
@@ -2446,12 +2674,12 @@
         <v>#N/A</v>
       </c>
       <c r="E76" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B77" s="12"/>
       <c r="C77" s="13"/>
@@ -2460,12 +2688,12 @@
         <v>#N/A</v>
       </c>
       <c r="E77" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B78" s="12"/>
       <c r="C78" s="13"/>
@@ -2474,12 +2702,12 @@
         <v>#N/A</v>
       </c>
       <c r="E78" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B79" s="12"/>
       <c r="C79" s="13"/>
@@ -2488,12 +2716,12 @@
         <v>#N/A</v>
       </c>
       <c r="E79" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B80" s="12"/>
       <c r="C80" s="13"/>
@@ -2502,36 +2730,36 @@
         <v>#N/A</v>
       </c>
       <c r="E80" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="82" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E82" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="83" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E83" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E84" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E85" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="D2:D80">
-    <cfRule type="duplicateValues" dxfId="1" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E80">
-    <cfRule type="duplicateValues" dxfId="0" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2550,11 +2778,11 @@
   <sheetPr>
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A2:K19"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2574,49 +2802,49 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" t="s">
-        <v>115</v>
-      </c>
-      <c r="D1" t="s">
-        <v>90</v>
-      </c>
       <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" t="s">
         <v>110</v>
       </c>
-      <c r="F1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" t="s">
-        <v>80</v>
-      </c>
-      <c r="H1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>111</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>112</v>
-      </c>
-      <c r="K1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" s="7" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -2627,13 +2855,13 @@
         <v>CL_ST_01A.ttl</v>
       </c>
       <c r="F2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
         <v>91</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>92</v>
-      </c>
-      <c r="H2" t="s">
-        <v>93</v>
       </c>
       <c r="I2" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -2646,14 +2874,14 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" s="7" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -2664,13 +2892,13 @@
         <v>CL_ST_01B.ttl</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I3" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -2683,14 +2911,14 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="7" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -2701,13 +2929,13 @@
         <v>CL_ST_01C.ttl</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I4" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -2720,14 +2948,14 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B5" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -2738,13 +2966,13 @@
         <v>CL_ST_01D.ttl</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I5" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -2755,19 +2983,19 @@
         <v>cwa,CL_ST_01,CL_ST_01D.ttl,error</v>
       </c>
       <c r="K5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B6" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -2778,13 +3006,13 @@
         <v>CL_ST_01E.ttl</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I6" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -2795,19 +3023,19 @@
         <v>cwa,CL_ST_01,CL_ST_01E.ttl,error</v>
       </c>
       <c r="K6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B7" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with exactly one stereotype.</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -2818,13 +3046,13 @@
         <v>CL_ST_01F.ttl</v>
       </c>
       <c r="F7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I7" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -2835,19 +3063,19 @@
         <v>cwa,CL_ST_01,CL_ST_01F.ttl,error</v>
       </c>
       <c r="K7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B8" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with stereotypes of the OntoUML profile.</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -2858,13 +3086,13 @@
         <v>CL_ST_02A.ttl</v>
       </c>
       <c r="F8" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" t="s">
         <v>91</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>92</v>
-      </c>
-      <c r="H8" t="s">
-        <v>93</v>
       </c>
       <c r="I8" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -2877,14 +3105,14 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B9" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with stereotypes of the OntoUML profile.</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -2895,13 +3123,13 @@
         <v>CL_ST_02B.ttl</v>
       </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I9" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -2914,14 +3142,14 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B10" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with stereotypes of the OntoUML profile.</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D10" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -2932,13 +3160,13 @@
         <v>CL_ST_02C.ttl</v>
       </c>
       <c r="F10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I10" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -2951,14 +3179,14 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with stereotypes of the OntoUML profile.</v>
       </c>
       <c r="C11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D11" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -2969,13 +3197,13 @@
         <v>CL_ST_02D.ttl</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I11" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -2986,19 +3214,19 @@
         <v>cwa,CL_ST_02,CL_ST_02D.ttl,error</v>
       </c>
       <c r="K11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with stereotypes of the OntoUML profile.</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D12" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -3009,13 +3237,13 @@
         <v>CL_ST_02E.ttl</v>
       </c>
       <c r="F12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I12" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -3026,19 +3254,19 @@
         <v>cwa,CL_ST_02,CL_ST_02E.ttl,valid</v>
       </c>
       <c r="K12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B13" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class must be decorated with stereotypes of the OntoUML profile.</v>
       </c>
       <c r="C13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -3049,13 +3277,13 @@
         <v>CL_ST_02F.ttl</v>
       </c>
       <c r="F13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I13" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -3066,19 +3294,19 @@
         <v>cwa,CL_ST_02,CL_ST_02F.ttl,error</v>
       </c>
       <c r="K13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B14" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
       </c>
       <c r="C14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D14" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -3089,13 +3317,13 @@
         <v>CL_EN_01A.ttl</v>
       </c>
       <c r="F14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I14" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -3108,14 +3336,14 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B15" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
       </c>
       <c r="C15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D15" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -3126,13 +3354,13 @@
         <v>CL_EN_01B.ttl</v>
       </c>
       <c r="F15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I15" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -3145,14 +3373,14 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
       </c>
       <c r="C16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D16" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -3163,13 +3391,13 @@
         <v>CL_EN_01C.ttl</v>
       </c>
       <c r="F16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I16" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -3180,16 +3408,16 @@
         <v>cwa,CL_EN_01,CL_EN_01C.ttl,valid</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D17" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -3200,13 +3428,13 @@
         <v>CL_EN_01D.ttl</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I17" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -3217,16 +3445,16 @@
         <v>cwa,CL_EN_01,CL_EN_01D.ttl,valid</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B18" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D18" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -3237,13 +3465,13 @@
         <v>CL_EN_01E.ttl</v>
       </c>
       <c r="F18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I18" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -3254,16 +3482,16 @@
         <v>cwa,CL_EN_01,CL_EN_01E.ttl,error</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B19" t="str">
         <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
         <v>Every class decorated with the stereotype «enumeration» must not have attributes.</v>
       </c>
       <c r="C19" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D19" t="str">
         <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
@@ -3274,13 +3502,13 @@
         <v>CL_EN_01F.ttl</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I19" t="str">
         <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
@@ -3291,23 +3519,254 @@
         <v>cwa,CL_EN_01,CL_EN_01F.ttl,error</v>
       </c>
     </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" s="16" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class having enumeration literals must be decorated with the stereotype enumeration.</v>
+      </c>
+      <c r="C20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="16" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL_EN_02A</v>
+      </c>
+      <c r="E20" s="16" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL_EN_02A.ttl</v>
+      </c>
+      <c r="F20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" t="s">
+        <v>97</v>
+      </c>
+      <c r="I20" s="16" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL_EN_02,CL_EN_02A.ttl,valid</v>
+      </c>
+      <c r="J20" s="16" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL_EN_02,CL_EN_02A.ttl,valid</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" s="16" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class having enumeration literals must be decorated with the stereotype enumeration.</v>
+      </c>
+      <c r="C21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="16" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL_EN_02B</v>
+      </c>
+      <c r="E21" s="16" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL_EN_02B.ttl</v>
+      </c>
+      <c r="F21" t="s">
+        <v>151</v>
+      </c>
+      <c r="G21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="16" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL_EN_02,CL_EN_02B.ttl,warning</v>
+      </c>
+      <c r="J21" s="16" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL_EN_02,CL_EN_02B.ttl,error</v>
+      </c>
+      <c r="K21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" s="16" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class having enumeration literals must be decorated with the stereotype enumeration.</v>
+      </c>
+      <c r="C22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="16" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL_EN_02C</v>
+      </c>
+      <c r="E22" s="16" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL_EN_02C.ttl</v>
+      </c>
+      <c r="F22" t="s">
+        <v>147</v>
+      </c>
+      <c r="G22" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" t="s">
+        <v>97</v>
+      </c>
+      <c r="I22" s="16" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL_EN_02,CL_EN_02C.ttl,valid</v>
+      </c>
+      <c r="J22" s="16" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL_EN_02,CL_EN_02C.ttl,valid</v>
+      </c>
+      <c r="K22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" s="16" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class having enumeration literals must be decorated with the stereotype enumeration.</v>
+      </c>
+      <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="16" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL_EN_02D</v>
+      </c>
+      <c r="E23" s="16" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL_EN_02D.ttl</v>
+      </c>
+      <c r="F23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G23" t="s">
+        <v>92</v>
+      </c>
+      <c r="H23" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="16" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL_EN_02,CL_EN_02D.ttl,error</v>
+      </c>
+      <c r="J23" s="16" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL_EN_02,CL_EN_02D.ttl,error</v>
+      </c>
+      <c r="K23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="16" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class having enumeration literals must be decorated with the stereotype enumeration.</v>
+      </c>
+      <c r="C24" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="16" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL_EN_02E</v>
+      </c>
+      <c r="E24" s="16" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL_EN_02E.ttl</v>
+      </c>
+      <c r="F24" t="s">
+        <v>143</v>
+      </c>
+      <c r="G24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H24" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="16" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL_EN_02,CL_EN_02E.ttl,warning</v>
+      </c>
+      <c r="J24" s="16" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL_EN_02,CL_EN_02E.ttl,error</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="16" t="str">
+        <f>VLOOKUP(TabImp[[#This Row],[Rule Code]],TabRules[[#All],[Rule Code]:[Description]],2,FALSE)</f>
+        <v>Every class having enumeration literals must be decorated with the stereotype enumeration.</v>
+      </c>
+      <c r="C25" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="16" t="str">
+        <f>TabImp[[#This Row],[Rule Code]]&amp;TabImp[[#This Row],[Situation ID]]</f>
+        <v>CL_EN_02F</v>
+      </c>
+      <c r="E25" s="16" t="str">
+        <f>TabImp[[#This Row],[Situation Code]]&amp;".ttl"</f>
+        <v>CL_EN_02F.ttl</v>
+      </c>
+      <c r="F25" t="s">
+        <v>144</v>
+      </c>
+      <c r="G25" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" t="s">
+        <v>97</v>
+      </c>
+      <c r="I25" s="16" t="str">
+        <f>"owa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[OWA Level]])</f>
+        <v>owa,CL_EN_02,CL_EN_02F.ttl,valid</v>
+      </c>
+      <c r="J25" s="16" t="str">
+        <f>"cwa"&amp;","&amp;TabImp[[#This Row],[Rule Code]]&amp;","&amp;TabImp[[#This Row],[Test File]]&amp;","&amp;LOWER(TabImp[[#This Row],[CWA Level]])</f>
+        <v>cwa,CL_EN_02,CL_EN_02F.ttl,valid</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:E19">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  <conditionalFormatting sqref="D2:E25">
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:H19">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+  <conditionalFormatting sqref="G2:H210">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Valid"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Warning"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H19" xr:uid="{88F4C713-6BF6-49A8-982F-7D1643817146}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:H25" xr:uid="{88F4C713-6BF6-49A8-982F-7D1643817146}">
       <formula1>"Valid,Error,Warning"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>